<commit_message>
data: add 2023-05-23 notices
</commit_message>
<xml_diff>
--- a/data/position_notices/2023-05-20.xlsx
+++ b/data/position_notices/2023-05-20.xlsx
@@ -464,41 +464,41 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>股票名称</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>股票代码</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>公告标题</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>公告日期</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>公告发布时间</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>公告附件</t>
         </is>
@@ -530,7 +530,7 @@
           <t>2023-05-22 19:45:41:000</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>https://pdf.dfcfw.com/pdf/H2_AN202305221587059456_1.pdf?1684784768000.pdf</t>
         </is>
@@ -562,7 +562,7 @@
           <t>2023-05-22 16:45:53:000</t>
         </is>
       </c>
-      <c r="F3" s="2" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>https://pdf.dfcfw.com/pdf/H2_AN202305221587050158_1.pdf?1684773965000.pdf</t>
         </is>
@@ -594,7 +594,7 @@
           <t>2023-05-22 20:31:37:000</t>
         </is>
       </c>
-      <c r="F4" s="2" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>https://pdf.dfcfw.com/pdf/H2_AN202305221587060191_1.pdf?1684787510000.pdf</t>
         </is>
@@ -626,7 +626,7 @@
           <t>2023-05-22 20:31:49:000</t>
         </is>
       </c>
-      <c r="F5" s="2" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>https://pdf.dfcfw.com/pdf/H2_AN202305221587060193_1.pdf?1684787510000.pdf</t>
         </is>
@@ -658,9 +658,9 @@
           <t>2023-05-22 20:31:37:000</t>
         </is>
       </c>
-      <c r="F6" s="2" t="inlineStr">
-        <is>
-          <t>https://pdf.dfcfw.com/pdf/H2_AN202305221587060187_1.pdf?1684787510000.pdf</t>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305221587060187_1.pdf?1684852281000.pdf</t>
         </is>
       </c>
     </row>
@@ -690,7 +690,7 @@
           <t>2023-05-22 17:57:22:000</t>
         </is>
       </c>
-      <c r="F7" s="2" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>https://pdf.dfcfw.com/pdf/H2_AN202305221587054049_1.pdf?1684778242000.pdf</t>
         </is>
@@ -699,79 +699,293 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>桐昆股份</t>
+          <t>ST广珠</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>601233</t>
+          <t>600382</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>桐昆股份:桐昆集团股份有限公司关于2023年度第三期超短期融资券发行结果的公告</t>
+          <t>ST广珠:广东明珠集团股份有限公司关于上海证券交易所《关于广东明珠集团股份有限公司2022年年度报告的信息披露监管问询函》的回复公告</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2023-05-23 00:00:00</t>
+          <t>2023-05-24 00:00:00</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-05-22 18:03:39:000</t>
-        </is>
-      </c>
-      <c r="F8" s="2" t="inlineStr">
-        <is>
-          <t>https://pdf.dfcfw.com/pdf/H2_AN202305221587054324_1.pdf?1684779087000.pdf</t>
+          <t>2023-05-23 17:58:40:000</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305231587099848_1.pdf?1684864746000.pdf</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>ST广珠</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>600382</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ST广珠:利安达会计师事务所(特殊普通合伙)关于上海证券交易所《关于广东明珠集团股份有限公司2022年年度报告的信息披露监管问询函》的回复</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2023-05-24 00:00:00</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2023-05-23 17:59:34:000</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305231587099849_1.pdf?1684865181000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ST澄星</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>600078</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ST澄星:江苏澄星磷化工股份有限公司关于延期回复上海证券交易所问询函的公告</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2023-05-24 00:00:00</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2023-05-23 19:09:44:000</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305231587106145_1.pdf?1684869000000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>桐昆股份</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>601233</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>桐昆股份:桐昆股份2022年年度股东大会会议资料</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2023-05-24 00:00:00</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2023-05-23 18:53:22:000</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305231587104385_1.pdf?1684868002000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>桐昆股份</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>601233</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>桐昆股份:桐昆集团股份有限公司关于召开2022年年度股东大会的提示性公告</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2023-05-24 00:00:00</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2023-05-23 17:44:44:000</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305231587099051_1.pdf?1684863901000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>桐昆股份</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>601233</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>桐昆股份:桐昆集团股份有限公司关于2023年度第三期超短期融资券发行结果的公告</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2023-05-23 00:00:00</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2023-05-22 18:03:39:000</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305221587054324_1.pdf?1684779087000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>三一重工</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>600031</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>三一重工:湖南启元律师事务所关于三一重工股份有限公司差异化分红的法律意见书</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2023-05-24 00:00:00</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2023-05-23 19:09:44:000</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305231587106141_1.pdf?1684868996000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>三一重工</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>600031</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>三一重工:三一重工股份有限公司2022年年度权益分派实施公告</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2023-05-24 00:00:00</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2023-05-23 19:09:44:000</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>https://pdf.dfcfw.com/pdf/H2_AN202305231587106143_1.pdf?1684869000000.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>海螺水泥</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>600585</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>海螺水泥:2022年年度股东大会会议资料</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>2023-05-23 00:00:00</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>2023-05-22 17:06:09:000</t>
         </is>
       </c>
-      <c r="F9" s="2" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>https://pdf.dfcfw.com/pdf/H2_AN202305221587051328_1.pdf?1684775173000.pdf</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F3" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F4" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F5" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F6" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F7" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F8" r:id="rId7"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F9" r:id="rId8"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -781,7 +995,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -869,30 +1083,75 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>桐昆股份</t>
+          <t>ST广珠</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>601233</t>
+          <t>600382</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>ST澄星</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>600078</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>桐昆股份</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>601233</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>三一重工</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>600031</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>海螺水泥</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>600585</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="C10" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>